<commit_message>
1/8/25 Company Code read as 362.0
</commit_message>
<xml_diff>
--- a/Allocations/Files for running Allocations/Chart of Accounts - Payroll.xlsx
+++ b/Allocations/Files for running Allocations/Chart of Accounts - Payroll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://springfertility.sharepoint.com/sites/accountingsharepoint/Shared Documents/AB-GV WIP/References - Z/References - Z/Payroll Allocation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorinan.kasilag\Programs\Spring-Python\Allocations\Files for running Allocations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{9C8B3DE1-4CE7-4382-8075-B5246499EE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FF47ED8-101D-45F7-B304-E5EFAC24E790}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915C0D88-2E7A-4A4D-8337-086ADBEDAD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2664EE9E-213A-4F81-8C48-3B2C2118C82E}"/>
+    <workbookView xWindow="4065" yWindow="4995" windowWidth="38700" windowHeight="14850" xr2:uid="{2664EE9E-213A-4F81-8C48-3B2C2118C82E}"/>
   </bookViews>
   <sheets>
     <sheet name="CHART of ACCOUNTS_Updated" sheetId="1" r:id="rId1"/>
@@ -69,21 +69,6 @@
     <t>OT</t>
   </si>
   <si>
-    <t>Medical Waiver</t>
-  </si>
-  <si>
-    <t>MEDICAL</t>
-  </si>
-  <si>
-    <t>DENTAL</t>
-  </si>
-  <si>
-    <t>VISION</t>
-  </si>
-  <si>
-    <t>LIFE</t>
-  </si>
-  <si>
     <t>Salaries and Wages</t>
   </si>
   <si>
@@ -103,6 +88,21 @@
   </si>
   <si>
     <t>DR BONUS DRAW</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>MEDICAL WAIVER</t>
   </si>
 </sst>
 </file>
@@ -272,9 +272,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -312,7 +312,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -418,7 +418,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -560,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,7 +574,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -595,43 +595,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -915,6 +915,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE5E0182BB4F9949ADFCEA3573795848" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="472a0c199ca28b3090b1dc2f1440b5b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="deb4e827-47a1-4ad9-a884-564aeea7cc89" xmlns:ns3="3b751711-07c7-4f61-9632-53893189454b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64c417c7e1b1d1f78af8d5fba48a2e29" ns2:_="" ns3:_="">
     <xsd:import namespace="deb4e827-47a1-4ad9-a884-564aeea7cc89"/>
@@ -1169,15 +1178,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B0710E-43E7-48DF-940A-4DEE200C25DE}">
   <ds:schemaRefs>
@@ -1191,6 +1191,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DB32677-A841-4614-9CFA-D34147D25199}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1635FB8-C33B-453F-B398-32DEC4DA2AC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1207,12 +1215,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DB32677-A841-4614-9CFA-D34147D25199}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>